<commit_message>
Updated progress and middle east v0.5
</commit_message>
<xml_diff>
--- a/src/Input_Files/characters.xlsx
+++ b/src/Input_Files/characters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python Scripts\imperator\ProvinceOrganizer\EP_ImperatorProvinceOrganizer\src\Input_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\EP_ImperatorProvinceOrganizer\src\Input_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49B1A6D-A62D-4E2C-BB05-36B6E07D884E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7A1091-12B3-4674-BBE1-754C56810BA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="1725" windowWidth="21600" windowHeight="10800" xr2:uid="{E5B2FA9E-FCEB-4F64-AA77-9CDFE63EBBF9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E5B2FA9E-FCEB-4F64-AA77-9CDFE63EBBF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="161">
   <si>
     <t>RGB</t>
   </si>
@@ -382,13 +382,148 @@
   </si>
   <si>
     <t>1399.1.13</t>
+  </si>
+  <si>
+    <t>CKU_ak_koyunlu_1</t>
+  </si>
+  <si>
+    <t>(31, 49, 138)</t>
+  </si>
+  <si>
+    <t>Jahangir bin Ali</t>
+  </si>
+  <si>
+    <t>1414.1.1</t>
+  </si>
+  <si>
+    <t>dynn_ak_koyunlu</t>
+  </si>
+  <si>
+    <t>CKU_trebizond_1</t>
+  </si>
+  <si>
+    <t>(40, 164, 157)</t>
+  </si>
+  <si>
+    <t>Ioannes</t>
+  </si>
+  <si>
+    <t>1403.1.1</t>
+  </si>
+  <si>
+    <t>dynn_komnenos</t>
+  </si>
+  <si>
+    <t>CKU_kara_koyunlu_1</t>
+  </si>
+  <si>
+    <t>(54, 117, 136)</t>
+  </si>
+  <si>
+    <t>Isfahan</t>
+  </si>
+  <si>
+    <t>1410.1.1</t>
+  </si>
+  <si>
+    <t>dynn_kara_koyunlu</t>
+  </si>
+  <si>
+    <t>CKU_bitlis_1</t>
+  </si>
+  <si>
+    <t>(205, 110, 47)</t>
+  </si>
+  <si>
+    <t>Bidlo</t>
+  </si>
+  <si>
+    <t>1421.1.1</t>
+  </si>
+  <si>
+    <t>dynn_rojaki</t>
+  </si>
+  <si>
+    <t>CKU_kharabakh_1</t>
+  </si>
+  <si>
+    <t>(117, 167, 117)</t>
+  </si>
+  <si>
+    <t>Albast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1425.1.1 </t>
+  </si>
+  <si>
+    <t>dynn_hasan_jalalyan</t>
+  </si>
+  <si>
+    <t>CKU_hakkari_1</t>
+  </si>
+  <si>
+    <t>(107, 159, 136)</t>
+  </si>
+  <si>
+    <t>Asad al-din Zarin</t>
+  </si>
+  <si>
+    <t>1412.1.1</t>
+  </si>
+  <si>
+    <t>dynn_cang</t>
+  </si>
+  <si>
+    <t>CKU_jalair_1</t>
+  </si>
+  <si>
+    <t>(162, 165, 193)</t>
+  </si>
+  <si>
+    <t>Hussain bin Ala-ud-Daulah Ahmed</t>
+  </si>
+  <si>
+    <t>1407.1.1</t>
+  </si>
+  <si>
+    <t>dynn_jalayir</t>
+  </si>
+  <si>
+    <t>CKU_mushasha_1</t>
+  </si>
+  <si>
+    <t>(140, 102, 152)</t>
+  </si>
+  <si>
+    <t>Muhammed</t>
+  </si>
+  <si>
+    <t>1422.1.1</t>
+  </si>
+  <si>
+    <t>dynn_falah</t>
+  </si>
+  <si>
+    <t>CKU_hisn_kayfa_1</t>
+  </si>
+  <si>
+    <t>(234, 179, 30)</t>
+  </si>
+  <si>
+    <t>Salih Salah ad-Din</t>
+  </si>
+  <si>
+    <t>1411.1.1</t>
+  </si>
+  <si>
+    <t>dynn_ayyubid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -398,6 +533,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202122"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -423,8 +565,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -739,41 +882,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{400C5842-DB98-492E-993D-80D39F62EB82}">
-  <dimension ref="A1:BC14"/>
+  <dimension ref="A1:BC23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E14"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="5.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -940,7 +1083,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -963,7 +1106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -983,7 +1126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1003,7 +1146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1023,7 +1166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -1043,7 +1186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -1063,7 +1206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -1083,7 +1226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -1103,7 +1246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1144,7 +1287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1188,7 +1331,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1232,7 +1375,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1273,7 +1416,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1312,6 +1455,201 @@
       </c>
       <c r="T14">
         <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" t="s">
+        <v>118</v>
+      </c>
+      <c r="E15" t="s">
+        <v>119</v>
+      </c>
+      <c r="H15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" t="s">
+        <v>123</v>
+      </c>
+      <c r="E16" t="s">
+        <v>124</v>
+      </c>
+      <c r="H16" t="s">
+        <v>27</v>
+      </c>
+      <c r="T16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>126</v>
+      </c>
+      <c r="B17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" t="s">
+        <v>128</v>
+      </c>
+      <c r="E17" t="s">
+        <v>129</v>
+      </c>
+      <c r="H17" t="s">
+        <v>27</v>
+      </c>
+      <c r="T17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" t="s">
+        <v>133</v>
+      </c>
+      <c r="E18" t="s">
+        <v>134</v>
+      </c>
+      <c r="G18" t="s">
+        <v>127</v>
+      </c>
+      <c r="H18" t="s">
+        <v>27</v>
+      </c>
+      <c r="T18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>136</v>
+      </c>
+      <c r="B19" t="s">
+        <v>137</v>
+      </c>
+      <c r="C19" t="s">
+        <v>138</v>
+      </c>
+      <c r="E19" t="s">
+        <v>139</v>
+      </c>
+      <c r="G19" t="s">
+        <v>127</v>
+      </c>
+      <c r="H19" t="s">
+        <v>27</v>
+      </c>
+      <c r="T19" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>141</v>
+      </c>
+      <c r="B20" t="s">
+        <v>142</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E20" t="s">
+        <v>144</v>
+      </c>
+      <c r="G20" t="s">
+        <v>127</v>
+      </c>
+      <c r="H20" t="s">
+        <v>27</v>
+      </c>
+      <c r="T20" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>146</v>
+      </c>
+      <c r="B21" t="s">
+        <v>147</v>
+      </c>
+      <c r="C21" t="s">
+        <v>148</v>
+      </c>
+      <c r="E21" t="s">
+        <v>149</v>
+      </c>
+      <c r="G21" t="s">
+        <v>127</v>
+      </c>
+      <c r="H21" t="s">
+        <v>27</v>
+      </c>
+      <c r="T21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>151</v>
+      </c>
+      <c r="B22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C22" t="s">
+        <v>153</v>
+      </c>
+      <c r="E22" t="s">
+        <v>154</v>
+      </c>
+      <c r="G22" t="s">
+        <v>127</v>
+      </c>
+      <c r="H22" t="s">
+        <v>27</v>
+      </c>
+      <c r="T22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>156</v>
+      </c>
+      <c r="B23" t="s">
+        <v>157</v>
+      </c>
+      <c r="C23" t="s">
+        <v>158</v>
+      </c>
+      <c r="E23" t="s">
+        <v>159</v>
+      </c>
+      <c r="H23" t="s">
+        <v>27</v>
+      </c>
+      <c r="T23" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>